<commit_message>
Updated project bubble to the draft - Migration plan
</commit_message>
<xml_diff>
--- a/Workshop 3/e. Project Prioritization - breakup 1.xlsx
+++ b/Workshop 3/e. Project Prioritization - breakup 1.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Project Prioritization" sheetId="1" r:id="rId1"/>
+    <sheet name="ROI - Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="Project Bubble" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>Project Initiatives</t>
   </si>
@@ -151,13 +152,52 @@
     <t>Savings</t>
   </si>
   <si>
-    <t>Expences</t>
-  </si>
-  <si>
     <t>Capital Cost (Development)</t>
   </si>
   <si>
     <t>Capital Cost (Infrastructure)</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>VCMS</t>
+  </si>
+  <si>
+    <t>SCBS</t>
+  </si>
+  <si>
+    <t>ShipTrack</t>
+  </si>
+  <si>
+    <t>ESB</t>
+  </si>
+  <si>
+    <t>MQ-HRS</t>
+  </si>
+  <si>
+    <t>MQ-AFIS</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>MR</t>
   </si>
 </sst>
 </file>
@@ -195,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,24 +256,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -256,11 +302,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -270,13 +526,34 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,6 +569,538 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="900"/>
+              <a:t>* Project Size</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="900" baseline="0"/>
+              <a:t> in Man Hrs</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="900"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82314930027639077"/>
+          <c:y val="0.96746069327796869"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Project Bubble'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$3</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>SCBS</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$4</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>VCMS</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$5</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>ShipTrack</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$6</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>ESB</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$7</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>MQ-HRS</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$8</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>MQ-AFIS</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$9</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>IE</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$10</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>WP</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>'Project Bubble'!$A$11</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>MR</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="700" b="1"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Project Bubble'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Project Bubble'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>64800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'Project Bubble'!$D$3:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2880</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>640</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="111352448"/>
+        <c:axId val="111395584"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="111352448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Project Risk (Dependency)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111395584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="111395584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Project Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111352448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,49 +1719,50 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="24" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7">
         <f>20000+35000</f>
         <v>55000</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="8">
         <v>0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="8">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="8">
         <v>0</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="10">
         <f>100800+134400 +33600 +16800 +16800 +67200</f>
         <v>369600</v>
       </c>
@@ -965,15 +1775,15 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="10">
         <f>10000</f>
         <v>10000</v>
       </c>
@@ -989,16 +1799,16 @@
         <f>10000</f>
         <v>10000</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="11">
         <f>10000</f>
         <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="10">
         <v>0</v>
       </c>
       <c r="C6" s="4">
@@ -1010,40 +1820,307 @@
         <v>182400</v>
       </c>
       <c r="E6" s="4">
-        <f>64800 +43200 +14400 + 60000</f>
-        <v>182400</v>
-      </c>
-      <c r="F6" s="4">
+        <f>64800 +43200 +14400 + 80000</f>
+        <v>202400</v>
+      </c>
+      <c r="F6" s="11">
         <f>64800 +43200 +14400 + 100000</f>
         <v>222400</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="A7" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="12">
         <f>B3+B4+B5-B6</f>
         <v>434600</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <f>B7+C5-C6</f>
         <v>282200</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <f t="shared" ref="D7:F7" si="0">C7+D5-D6</f>
         <v>109800</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>-62600</v>
-      </c>
-      <c r="F7" s="9">
+        <v>-82600</v>
+      </c>
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
-        <v>-275000</v>
+        <v>-295000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="14">
+        <f>IF(B7&gt;0,0,-B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="15">
+        <f t="shared" ref="C8:F8" si="1">IF(C7&gt;0,0,-C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <f t="shared" si="1"/>
+        <v>82600</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="1"/>
+        <v>295000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="28">
+        <v>64800</v>
+      </c>
+      <c r="D3" s="28">
+        <v>2880</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="28">
+        <v>43200</v>
+      </c>
+      <c r="D4" s="28">
+        <v>3840</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="28">
+        <v>14400</v>
+      </c>
+      <c r="D5" s="28">
+        <v>960</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="29">
+        <v>1</v>
+      </c>
+      <c r="C6" s="28">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="28">
+        <v>480</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="29">
+        <v>8</v>
+      </c>
+      <c r="C7" s="30">
+        <v>5000</v>
+      </c>
+      <c r="D7" s="28">
+        <v>240</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="29">
+        <v>9</v>
+      </c>
+      <c r="C8" s="30">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="28">
+        <v>240</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="29">
+        <v>5</v>
+      </c>
+      <c r="C9" s="30">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="30">
+        <v>640</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="29">
+        <v>6</v>
+      </c>
+      <c r="C10" s="30">
+        <v>10000</v>
+      </c>
+      <c r="D10" s="30">
+        <v>640</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="29">
+        <v>7</v>
+      </c>
+      <c r="C11" s="30">
+        <v>10000</v>
+      </c>
+      <c r="D11" s="30">
+        <v>640</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>